<commit_message>
add dependencies and refine code
</commit_message>
<xml_diff>
--- a/src/main/resources/template/import_template.xlsx
+++ b/src/main/resources/template/import_template.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F85D229-05F9-4D59-8614-3ED77D7B410B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="110" windowWidth="14810" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,21 +17,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
-  <si>
-    <t>序号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>研究人员姓名</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>证件类型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>证件号码</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>姓名</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>年龄</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -38,95 +31,26 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>年龄</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>技术职称</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>研究任务及分工（限100字）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>全时率</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>所在单位</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>张三</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>男</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>李四</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>中国居民身份证</t>
-  </si>
-  <si>
-    <t>其他</t>
-  </si>
-  <si>
-    <t>女</t>
-  </si>
-  <si>
-    <t>总工1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>总工2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>20</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>男</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>17</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xxxxxxxxxxxxx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xxxxxxxxxxxxxx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xxx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xxxx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xxx</t>
+    <t>a</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -144,7 +68,7 @@
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="14"/>
       <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <family val="3"/>
@@ -166,12 +90,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -180,10 +119,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -193,6 +132,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -241,7 +183,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -274,9 +216,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -309,6 +268,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -484,26 +460,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="5.26953125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.90625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="24.453125" style="2" customWidth="1"/>
-    <col min="5" max="7" width="9" style="2"/>
-    <col min="8" max="8" width="26.7265625" style="2" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.36328125" style="2" customWidth="1"/>
+    <col min="1" max="3" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -513,114 +482,43 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" s="2">
+        <v>17</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B3" s="2">
+        <v>227</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>2</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C1:C1048576">
-      <formula1>"中国居民身份证,其他"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E1:E1048576">
-      <formula1>"男,女"</formula1>
-    </dataValidation>
-  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -628,12 +526,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>